<commit_message>
Correção de velocidade; Remoção de casos muito curtos; Consideração de múltiplos p3d; Limpeza da pasta de output.
</commit_message>
<xml_diff>
--- a/Input/tabela_Aframax.xlsx
+++ b/Input/tabela_Aframax.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMH\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduardo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="11445"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Ordem</t>
   </si>
   <si>
     <t>propeller_demanded_0</t>
+  </si>
+  <si>
+    <t>Aframax</t>
+  </si>
+  <si>
+    <t>Suezmax</t>
+  </si>
+  <si>
+    <t>Aframax Casos Estranhos</t>
+  </si>
+  <si>
+    <t>L280B50T17</t>
   </si>
 </sst>
 </file>
@@ -347,103 +359,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:E12"/>
+  <dimension ref="D1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>-4</v>
       </c>
       <c r="E3">
         <v>-1096.68</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>-1420.0200000000002</v>
+      </c>
+      <c r="H3">
+        <v>-74</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>-3</v>
       </c>
       <c r="E4">
         <v>-663.42</v>
       </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>-858.48</v>
+      </c>
+      <c r="H4">
+        <v>-58</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>-2</v>
       </c>
       <c r="E5">
         <v>-338.48</v>
       </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>-631.12000000000012</v>
+      </c>
+      <c r="H5">
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>-1</v>
       </c>
       <c r="E6">
         <v>-121.85</v>
       </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>-438.06000000000006</v>
+      </c>
+      <c r="H6">
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>95</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
         <v>203.09000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>730.1</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9">
         <v>564.14</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1051.54</v>
+      </c>
+      <c r="G9">
+        <v>400</v>
+      </c>
+      <c r="H9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10">
         <v>1105.71</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1431.78</v>
+      </c>
+      <c r="G10">
+        <v>800</v>
+      </c>
+      <c r="H10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11">
         <v>1827.7999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>2366.7000000000003</v>
+      </c>
+      <c r="H11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12">
         <v>2256.54</v>
+      </c>
+      <c r="F12">
+        <v>2921.3800000000006</v>
+      </c>
+      <c r="H12">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>